<commit_message>
Player names can't have spaces
</commit_message>
<xml_diff>
--- a/great_war_1916.xlsx
+++ b/great_war_1916.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="26820" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="5940" yWindow="0" windowWidth="26820" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -1363,12 +1363,6 @@
     <t>Germans</t>
   </si>
   <si>
-    <t>Imperial German Afrika</t>
-  </si>
-  <si>
-    <t>British Commonwealth</t>
-  </si>
-  <si>
     <t>Rhodesia</t>
   </si>
   <si>
@@ -1396,9 +1390,6 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>French Colonial Africa</t>
-  </si>
-  <si>
     <t>French West Africa</t>
   </si>
   <si>
@@ -1565,6 +1556,15 @@
   </si>
   <si>
     <t>German E. Afrika</t>
+  </si>
+  <si>
+    <t>British-Commonwealth</t>
+  </si>
+  <si>
+    <t>French-Colonial-Africa</t>
+  </si>
+  <si>
+    <t>Imperial-German-Afrika</t>
   </si>
 </sst>
 </file>
@@ -2907,8 +2907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3063,7 +3063,7 @@
         <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3077,7 +3077,7 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3091,7 +3091,7 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -3105,7 +3105,7 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -3119,7 +3119,7 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -3133,7 +3133,7 @@
         <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -3141,13 +3141,13 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -3161,7 +3161,7 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3169,7 +3169,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>42</v>
@@ -3189,7 +3189,7 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -3203,7 +3203,7 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3217,7 +3217,7 @@
         <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3225,13 +3225,13 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -3245,7 +3245,7 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3259,7 +3259,7 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3273,7 +3273,7 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -3281,13 +3281,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -3301,7 +3301,7 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -3309,13 +3309,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -3323,7 +3323,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>42</v>
@@ -3331,13 +3331,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3345,13 +3345,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -3359,7 +3359,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>42</v>
@@ -3373,13 +3373,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D26">
         <v>4</v>
@@ -3393,7 +3393,7 @@
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -3401,13 +3401,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -3421,7 +3421,7 @@
         <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -3435,7 +3435,7 @@
         <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -3449,7 +3449,7 @@
         <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -3463,7 +3463,7 @@
         <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -3491,7 +3491,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -3505,7 +3505,7 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -3533,7 +3533,7 @@
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D37">
         <v>6</v>
@@ -3547,7 +3547,7 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -3555,13 +3555,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3572,7 +3572,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -3586,7 +3586,7 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -3600,7 +3600,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -3608,13 +3608,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -3628,7 +3628,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -3642,7 +3642,7 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -3670,7 +3670,7 @@
         <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -3684,7 +3684,7 @@
         <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -3712,7 +3712,7 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -3726,7 +3726,7 @@
         <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3740,7 +3740,7 @@
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -3754,7 +3754,7 @@
         <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -3768,7 +3768,7 @@
         <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -3782,7 +3782,7 @@
         <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -3798,7 +3798,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>42</v>
@@ -3812,13 +3812,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3832,7 +3832,7 @@
         <v>42</v>
       </c>
       <c r="C59" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -3840,13 +3840,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C60" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D60">
         <v>3</v>
@@ -3860,7 +3860,7 @@
         <v>42</v>
       </c>
       <c r="C61" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -3882,13 +3882,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C63" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -3902,7 +3902,7 @@
         <v>42</v>
       </c>
       <c r="C64" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -3916,7 +3916,7 @@
         <v>42</v>
       </c>
       <c r="C65" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -3930,7 +3930,7 @@
         <v>42</v>
       </c>
       <c r="C66" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -3938,13 +3938,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -3958,7 +3958,7 @@
         <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D68">
         <v>4</v>
@@ -3972,7 +3972,7 @@
         <v>42</v>
       </c>
       <c r="C69" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -3980,13 +3980,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>511</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C70" t="s">
         <v>514</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C70" t="s">
-        <v>447</v>
       </c>
       <c r="D70">
         <v>4</v>
@@ -4000,7 +4000,7 @@
         <v>42</v>
       </c>
       <c r="C71" t="s">
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -4014,7 +4014,7 @@
         <v>42</v>
       </c>
       <c r="C72" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -4028,7 +4028,7 @@
         <v>42</v>
       </c>
       <c r="C73" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D73">
         <v>4</v>
@@ -4042,7 +4042,7 @@
         <v>42</v>
       </c>
       <c r="C74" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -4050,7 +4050,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>42</v>
@@ -4064,13 +4064,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C76" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -4086,13 +4086,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C78" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D78">
         <v>6</v>
@@ -4106,7 +4106,7 @@
         <v>42</v>
       </c>
       <c r="C79" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -4120,7 +4120,7 @@
         <v>42</v>
       </c>
       <c r="C80" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -4134,7 +4134,7 @@
         <v>42</v>
       </c>
       <c r="C81" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -4148,7 +4148,7 @@
         <v>42</v>
       </c>
       <c r="C82" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D82">
         <v>5</v>
@@ -4162,7 +4162,7 @@
         <v>42</v>
       </c>
       <c r="C83" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D83">
         <v>2</v>
@@ -4176,7 +4176,7 @@
         <v>42</v>
       </c>
       <c r="C84" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D84">
         <v>10</v>
@@ -4184,13 +4184,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C85" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -4204,7 +4204,7 @@
         <v>42</v>
       </c>
       <c r="C86" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D86">
         <v>2</v>
@@ -4212,13 +4212,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C87" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D87">
         <v>4</v>
@@ -4226,13 +4226,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C88" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -4240,13 +4240,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C89" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -4254,13 +4254,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C90" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -4282,13 +4282,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C92" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -4302,7 +4302,7 @@
         <v>42</v>
       </c>
       <c r="C93" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -4316,7 +4316,7 @@
         <v>42</v>
       </c>
       <c r="C94" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D94">
         <v>2</v>
@@ -4330,7 +4330,7 @@
         <v>42</v>
       </c>
       <c r="C95" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -4344,7 +4344,7 @@
         <v>42</v>
       </c>
       <c r="C96" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D96">
         <v>10</v>
@@ -4358,7 +4358,7 @@
         <v>42</v>
       </c>
       <c r="C97" t="s">
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="D97">
         <v>2</v>
@@ -4380,13 +4380,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C99" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D99">
         <v>2</v>
@@ -4400,7 +4400,7 @@
         <v>42</v>
       </c>
       <c r="C100" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -4414,7 +4414,7 @@
         <v>42</v>
       </c>
       <c r="C101" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D101">
         <v>6</v>
@@ -4422,13 +4422,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C102" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D102">
         <v>2</v>
@@ -4442,7 +4442,7 @@
         <v>42</v>
       </c>
       <c r="C103" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D103">
         <v>2</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>42</v>
@@ -4464,13 +4464,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C105" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D105">
         <v>2</v>
@@ -4498,7 +4498,7 @@
         <v>42</v>
       </c>
       <c r="C107" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D107">
         <v>6</v>
@@ -4512,7 +4512,7 @@
         <v>42</v>
       </c>
       <c r="C108" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D108">
         <v>2</v>
@@ -4526,7 +4526,7 @@
         <v>42</v>
       </c>
       <c r="C109" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -4540,7 +4540,7 @@
         <v>42</v>
       </c>
       <c r="C110" t="s">
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="D110">
         <v>2</v>
@@ -4554,7 +4554,7 @@
         <v>42</v>
       </c>
       <c r="C111" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -4568,7 +4568,7 @@
         <v>42</v>
       </c>
       <c r="C112" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D112">
         <v>3</v>
@@ -4576,13 +4576,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C113" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -4596,7 +4596,7 @@
         <v>42</v>
       </c>
       <c r="C114" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -4604,13 +4604,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C115" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -4624,7 +4624,7 @@
         <v>42</v>
       </c>
       <c r="C116" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D116">
         <v>3</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>42</v>
@@ -4652,7 +4652,7 @@
         <v>42</v>
       </c>
       <c r="C118" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D118">
         <v>1</v>
@@ -4668,13 +4668,13 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C120" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -4688,7 +4688,7 @@
         <v>42</v>
       </c>
       <c r="C121" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D121">
         <v>1</v>
@@ -4702,7 +4702,7 @@
         <v>42</v>
       </c>
       <c r="C122" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -4710,13 +4710,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C123" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D123">
         <v>2</v>
@@ -4730,7 +4730,7 @@
         <v>42</v>
       </c>
       <c r="C124" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D124">
         <v>12</v>
@@ -4760,13 +4760,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C127" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D127">
         <v>6</v>
@@ -4780,7 +4780,7 @@
         <v>42</v>
       </c>
       <c r="C128" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D128">
         <v>6</v>
@@ -4802,7 +4802,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>42</v>
@@ -4822,7 +4822,7 @@
         <v>42</v>
       </c>
       <c r="C131" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D131">
         <v>3</v>
@@ -4836,7 +4836,7 @@
         <v>42</v>
       </c>
       <c r="C132" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D132">
         <v>1</v>
@@ -4858,13 +4858,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C134" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -4886,13 +4886,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B136" t="s">
         <v>42</v>
       </c>
       <c r="C136" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -4900,13 +4900,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B137" t="s">
         <v>42</v>
       </c>
       <c r="C137" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -4920,7 +4920,7 @@
         <v>42</v>
       </c>
       <c r="C138" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -4928,13 +4928,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B139" t="s">
         <v>42</v>
       </c>
       <c r="C139" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D139">
         <v>4</v>
@@ -4942,13 +4942,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B140" t="s">
         <v>42</v>
       </c>
       <c r="C140" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D140">
         <v>10</v>
@@ -4956,13 +4956,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B141" t="s">
         <v>42</v>
       </c>
       <c r="C141" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B187" t="s">
         <v>39</v>
@@ -6118,7 +6118,7 @@
         <v>42</v>
       </c>
       <c r="C284" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D284">
         <v>3</v>
@@ -6132,7 +6132,7 @@
         <v>42</v>
       </c>
       <c r="C285" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D285">
         <v>3</v>
@@ -6146,7 +6146,7 @@
         <v>42</v>
       </c>
       <c r="C286" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D286">
         <v>1</v>
@@ -6160,7 +6160,7 @@
         <v>42</v>
       </c>
       <c r="C287" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D287">
         <v>2</v>
@@ -6174,7 +6174,7 @@
         <v>42</v>
       </c>
       <c r="C288" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D288">
         <v>1</v>
@@ -6188,7 +6188,7 @@
         <v>42</v>
       </c>
       <c r="C289" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D289">
         <v>1</v>
@@ -6216,7 +6216,7 @@
         <v>42</v>
       </c>
       <c r="C291" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D291">
         <v>2</v>
@@ -6230,7 +6230,7 @@
         <v>42</v>
       </c>
       <c r="C292" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D292">
         <v>3</v>
@@ -6238,13 +6238,13 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C293" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D293">
         <v>3</v>
@@ -6258,7 +6258,7 @@
         <v>42</v>
       </c>
       <c r="C294" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D294">
         <v>2</v>
@@ -6272,7 +6272,7 @@
         <v>42</v>
       </c>
       <c r="C295" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D295">
         <v>2</v>
@@ -6300,7 +6300,7 @@
         <v>42</v>
       </c>
       <c r="C297" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -6314,7 +6314,7 @@
         <v>42</v>
       </c>
       <c r="C298" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D298">
         <v>2</v>
@@ -6328,7 +6328,7 @@
         <v>42</v>
       </c>
       <c r="C299" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D299">
         <v>2</v>
@@ -6336,13 +6336,13 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C300" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D300">
         <v>1</v>
@@ -6350,7 +6350,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>42</v>
@@ -6370,7 +6370,7 @@
         <v>42</v>
       </c>
       <c r="C302" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D302">
         <v>1</v>
@@ -6394,13 +6394,13 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C305" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D305">
         <v>6</v>
@@ -6408,7 +6408,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>42</v>
@@ -6428,7 +6428,7 @@
         <v>42</v>
       </c>
       <c r="C307" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D307">
         <v>6</v>
@@ -6458,7 +6458,7 @@
         <v>42</v>
       </c>
       <c r="C310" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D310">
         <v>4</v>
@@ -6634,7 +6634,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B332" t="s">
         <v>39</v>
@@ -7184,7 +7184,7 @@
         <v>42</v>
       </c>
       <c r="C400" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D400">
         <v>2</v>
@@ -7198,7 +7198,7 @@
         <v>42</v>
       </c>
       <c r="C401" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D401">
         <v>1</v>
@@ -7206,13 +7206,13 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B402" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C402" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D402">
         <v>2</v>
@@ -7220,13 +7220,13 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B403" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C403" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D403">
         <v>1</v>
@@ -7240,7 +7240,7 @@
         <v>42</v>
       </c>
       <c r="C404" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D404">
         <v>2</v>
@@ -7254,7 +7254,7 @@
         <v>42</v>
       </c>
       <c r="C405" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D405">
         <v>1</v>
@@ -7268,7 +7268,7 @@
         <v>42</v>
       </c>
       <c r="C406" t="s">
-        <v>447</v>
+        <v>514</v>
       </c>
       <c r="D406">
         <v>2</v>
@@ -7276,13 +7276,13 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B407" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C407" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D407">
         <v>3</v>
@@ -7296,7 +7296,7 @@
         <v>42</v>
       </c>
       <c r="C408" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D408">
         <v>1</v>
@@ -7310,7 +7310,7 @@
         <v>42</v>
       </c>
       <c r="C409" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D409">
         <v>6</v>
@@ -7324,7 +7324,7 @@
         <v>42</v>
       </c>
       <c r="C410" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D410">
         <v>1</v>
@@ -7338,7 +7338,7 @@
         <v>42</v>
       </c>
       <c r="C411" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D411">
         <v>1</v>
@@ -7352,7 +7352,7 @@
         <v>42</v>
       </c>
       <c r="C412" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D412">
         <v>1</v>
@@ -7360,13 +7360,13 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B413" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C413" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D413">
         <v>1</v>
@@ -7374,13 +7374,13 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B414" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C414" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D414">
         <v>3</v>
@@ -7394,7 +7394,7 @@
         <v>42</v>
       </c>
       <c r="C415" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="D415">
         <v>1</v>
@@ -7430,7 +7430,7 @@
         <v>42</v>
       </c>
       <c r="C418" t="s">
-        <v>458</v>
+        <v>513</v>
       </c>
       <c r="D418">
         <v>1</v>
@@ -7477,7 +7477,7 @@
         <v>42</v>
       </c>
       <c r="C422" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D422">
         <v>6</v>
@@ -7491,7 +7491,7 @@
         <v>42</v>
       </c>
       <c r="C423" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D423">
         <v>1</v>
@@ -7505,7 +7505,7 @@
         <v>42</v>
       </c>
       <c r="C424" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D424">
         <v>12</v>
@@ -7519,7 +7519,7 @@
         <v>42</v>
       </c>
       <c r="C425" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D425">
         <v>2</v>
@@ -7547,7 +7547,7 @@
         <v>42</v>
       </c>
       <c r="C427" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D427">
         <v>1</v>
@@ -7561,7 +7561,7 @@
         <v>42</v>
       </c>
       <c r="C428" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D428">
         <v>1</v>
@@ -7575,7 +7575,7 @@
         <v>42</v>
       </c>
       <c r="C429" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D429">
         <v>4</v>
@@ -7589,7 +7589,7 @@
         <v>42</v>
       </c>
       <c r="C430" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D430">
         <v>1</v>

</xml_diff>